<commit_message>
data, and exp updates
</commit_message>
<xml_diff>
--- a/RF_params.xlsx
+++ b/RF_params.xlsx
@@ -30,37 +30,37 @@
     <t>freq</t>
   </si>
   <si>
-    <t>[0, 00]</t>
-  </si>
-  <si>
-    <t>[-45, 45]</t>
-  </si>
-  <si>
-    <t>[0, 45]</t>
-  </si>
-  <si>
-    <t>[45, 45]</t>
-  </si>
-  <si>
     <t>[-45,0]</t>
   </si>
   <si>
-    <t>[45, 00]</t>
-  </si>
-  <si>
-    <t>[-45, -45]</t>
-  </si>
-  <si>
-    <t>[0,-45]</t>
-  </si>
-  <si>
-    <t>[45, -45]</t>
-  </si>
-  <si>
     <t>size</t>
   </si>
   <si>
     <t>[55, 55]</t>
+  </si>
+  <si>
+    <t>[-45, 40]</t>
+  </si>
+  <si>
+    <t>[0, 40]</t>
+  </si>
+  <si>
+    <t>[45, 40]</t>
+  </si>
+  <si>
+    <t>[0, 0]</t>
+  </si>
+  <si>
+    <t>[45, 0]</t>
+  </si>
+  <si>
+    <t>[-45, -40]</t>
+  </si>
+  <si>
+    <t>[0,-40]</t>
+  </si>
+  <si>
+    <t>[45, -40]</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,7 +382,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" activeCellId="1" sqref="D4:D10 D3:D10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -398,12 +398,12 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0.03</v>
@@ -412,12 +412,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0.03</v>
@@ -426,12 +426,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.03</v>
@@ -440,12 +440,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0.03</v>
@@ -454,12 +454,12 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.03</v>
@@ -468,12 +468,12 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0.03</v>
@@ -482,12 +482,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.03</v>
@@ -496,12 +496,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0.03</v>
@@ -510,12 +510,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.03</v>
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>